<commit_message>
Files until month 4
</commit_message>
<xml_diff>
--- a/data/data_sizes.xlsx
+++ b/data/data_sizes.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Uni\TFG\Proyecto-TFG-Reddit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47148F93-5629-4858-81BD-9F6B805BDB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D34C0A2-131A-4091-9B9D-998C97D4035C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="15600" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>abuse</t>
   </si>
@@ -73,6 +83,9 @@
   </si>
   <si>
     <t>Month</t>
+  </si>
+  <si>
+    <t>Median</t>
   </si>
 </sst>
 </file>
@@ -96,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +128,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -128,17 +153,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N16"/>
+  <dimension ref="B1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="C12" sqref="C12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,327 +457,492 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
     <row r="2" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>2</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="6">
         <v>3</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="6">
         <v>4</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="6">
         <v>5</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="6">
         <v>6</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="6">
         <v>7</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="6">
         <v>8</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="6">
         <v>9</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="6">
         <v>10</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="6">
         <v>11</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="6">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5">
+      <c r="C3" s="2">
+        <v>1144</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1170</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1386</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1585</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2">
         <v>1240</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5">
+      <c r="C4" s="2">
+        <v>6233</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5905</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5986</v>
+      </c>
+      <c r="F4" s="2">
+        <v>6025</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2">
         <v>6138</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5">
+      <c r="C5" s="2">
+        <v>305</v>
+      </c>
+      <c r="D5" s="2">
+        <v>316</v>
+      </c>
+      <c r="E5" s="2">
+        <v>395</v>
+      </c>
+      <c r="F5" s="2">
+        <v>368</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2">
         <v>439</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5">
+      <c r="C6" s="2">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2">
+        <v>66</v>
+      </c>
+      <c r="E6" s="2">
+        <v>100</v>
+      </c>
+      <c r="F6" s="2">
+        <v>90</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2">
         <v>94</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5">
+      <c r="C7" s="2">
+        <v>9858</v>
+      </c>
+      <c r="D7" s="2">
+        <v>10099</v>
+      </c>
+      <c r="E7" s="2">
+        <v>10907</v>
+      </c>
+      <c r="F7" s="2">
+        <v>11081</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2">
         <v>11317</v>
       </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5">
+      <c r="C8" s="2">
+        <v>2101</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2482</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2568</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2518</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2">
         <v>3270</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5">
+      <c r="C9" s="2">
+        <v>8079</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7689</v>
+      </c>
+      <c r="E9" s="2">
+        <v>8167</v>
+      </c>
+      <c r="F9" s="2">
+        <v>7930</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2">
         <v>6723</v>
       </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5">
+      <c r="C10" s="2">
+        <v>1794</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1730</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1714</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1815</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2">
         <v>2281</v>
       </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5">
+      <c r="C11" s="2">
+        <v>266</v>
+      </c>
+      <c r="D11" s="2">
+        <v>270</v>
+      </c>
+      <c r="E11" s="2">
+        <v>330</v>
+      </c>
+      <c r="F11" s="2">
+        <v>404</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2">
         <v>410</v>
       </c>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5">
+      <c r="C12" s="2">
+        <v>17583</v>
+      </c>
+      <c r="D12" s="2">
+        <v>17138</v>
+      </c>
+      <c r="E12" s="2">
+        <v>18455</v>
+      </c>
+      <c r="F12" s="2">
+        <v>19158</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2">
         <v>17476</v>
       </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5">
+      <c r="C13" s="2">
+        <v>1817</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1716</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1605</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1581</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2">
         <v>2087</v>
       </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5">
+      <c r="C14" s="2">
+        <v>22021</v>
+      </c>
+      <c r="D14" s="2">
+        <v>22477</v>
+      </c>
+      <c r="E14" s="2">
+        <v>23031</v>
+      </c>
+      <c r="F14" s="2">
+        <v>24703</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2">
         <v>23707</v>
       </c>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5">
+      <c r="C15" s="2">
+        <v>1477</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1507</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1985</v>
+      </c>
+      <c r="F15" s="2">
+        <v>2269</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2">
         <v>2099</v>
       </c>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5">
+      <c r="C16" s="2">
+        <v>10702</v>
+      </c>
+      <c r="D16" s="2">
+        <v>9157</v>
+      </c>
+      <c r="E16" s="2">
+        <v>10220</v>
+      </c>
+      <c r="F16" s="2">
+        <v>9734</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2">
         <v>9421</v>
       </c>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <f>MEDIAN(C3:C16)</f>
+        <v>1959</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:N18" si="0">MEDIAN(D3:D16)</f>
+        <v>2106</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>2276.5</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>2393.5</v>
+      </c>
+      <c r="G18" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="H18" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="I18" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="J18" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>2775.5</v>
+      </c>
+      <c r="L18" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M18" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N18" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Remaining files and changes in counter
</commit_message>
<xml_diff>
--- a/data/data_sizes.xlsx
+++ b/data/data_sizes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Uni\TFG\Proyecto-TFG-Reddit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D34C0A2-131A-4091-9B9D-998C97D4035C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1177DA98-4E48-46E7-B5A3-305A326A434E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="15600" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,14 +157,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +448,7 @@
   <dimension ref="B1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:F12"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,59 +457,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
     </row>
     <row r="2" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="4">
         <v>2</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="4">
         <v>3</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="4">
         <v>4</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="4">
         <v>5</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="4">
         <v>6</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="4">
         <v>7</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="4">
         <v>8</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="4">
         <v>9</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="4">
         <v>10</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="4">
         <v>11</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="4">
         <v>12</v>
       </c>
     </row>
@@ -529,16 +529,30 @@
       <c r="F3" s="2">
         <v>1585</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="G3" s="2">
+        <v>1502</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1371</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1544</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1676</v>
+      </c>
       <c r="K3" s="2">
         <v>1240</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="L3" s="2">
+        <v>1433</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1534</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1679</v>
+      </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -556,16 +570,30 @@
       <c r="F4" s="2">
         <v>6025</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="G4" s="2">
+        <v>6497</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5868</v>
+      </c>
+      <c r="I4" s="2">
+        <v>6961</v>
+      </c>
+      <c r="J4" s="2">
+        <v>8361</v>
+      </c>
       <c r="K4" s="2">
         <v>6138</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="L4" s="2">
+        <v>6152</v>
+      </c>
+      <c r="M4" s="2">
+        <v>5853</v>
+      </c>
+      <c r="N4" s="2">
+        <v>6398</v>
+      </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -583,16 +611,30 @@
       <c r="F5" s="2">
         <v>368</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="G5" s="2">
+        <v>480</v>
+      </c>
+      <c r="H5" s="2">
+        <v>408</v>
+      </c>
+      <c r="I5" s="2">
+        <v>476</v>
+      </c>
+      <c r="J5" s="2">
+        <v>512</v>
+      </c>
       <c r="K5" s="2">
         <v>439</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="L5" s="2">
+        <v>479</v>
+      </c>
+      <c r="M5" s="2">
+        <v>487</v>
+      </c>
+      <c r="N5" s="2">
+        <v>585</v>
+      </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -610,16 +652,30 @@
       <c r="F6" s="2">
         <v>90</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="G6" s="2">
+        <v>120</v>
+      </c>
+      <c r="H6" s="2">
+        <v>97</v>
+      </c>
+      <c r="I6" s="2">
+        <v>116</v>
+      </c>
+      <c r="J6" s="2">
+        <v>122</v>
+      </c>
       <c r="K6" s="2">
         <v>94</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="L6" s="2">
+        <v>94</v>
+      </c>
+      <c r="M6" s="2">
+        <v>88</v>
+      </c>
+      <c r="N6" s="2">
+        <v>72</v>
+      </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -637,16 +693,30 @@
       <c r="F7" s="2">
         <v>11081</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="G7" s="2">
+        <v>12219</v>
+      </c>
+      <c r="H7" s="2">
+        <v>11567</v>
+      </c>
+      <c r="I7" s="2">
+        <v>13005</v>
+      </c>
+      <c r="J7" s="2">
+        <v>13978</v>
+      </c>
       <c r="K7" s="2">
         <v>11317</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="L7" s="2">
+        <v>12823</v>
+      </c>
+      <c r="M7" s="2">
+        <v>12975</v>
+      </c>
+      <c r="N7" s="2">
+        <v>13799</v>
+      </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
@@ -664,16 +734,30 @@
       <c r="F8" s="2">
         <v>2518</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="G8" s="2">
+        <v>2913</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2678</v>
+      </c>
+      <c r="I8" s="2">
+        <v>3387</v>
+      </c>
+      <c r="J8" s="2">
+        <v>3702</v>
+      </c>
       <c r="K8" s="2">
         <v>3270</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="L8" s="2">
+        <v>3935</v>
+      </c>
+      <c r="M8" s="2">
+        <v>4137</v>
+      </c>
+      <c r="N8" s="2">
+        <v>4194</v>
+      </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -691,16 +775,30 @@
       <c r="F9" s="2">
         <v>7930</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="G9" s="2">
+        <v>8431</v>
+      </c>
+      <c r="H9" s="2">
+        <v>7720</v>
+      </c>
+      <c r="I9" s="2">
+        <v>7994</v>
+      </c>
+      <c r="J9" s="2">
+        <v>8737</v>
+      </c>
       <c r="K9" s="2">
         <v>6723</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
+      <c r="L9" s="2">
+        <v>6584</v>
+      </c>
+      <c r="M9" s="2">
+        <v>6910</v>
+      </c>
+      <c r="N9" s="2">
+        <v>9023</v>
+      </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -718,16 +816,30 @@
       <c r="F10" s="2">
         <v>1815</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="G10" s="2">
+        <v>2340</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2191</v>
+      </c>
+      <c r="I10" s="2">
+        <v>2544</v>
+      </c>
+      <c r="J10" s="2">
+        <v>3563</v>
+      </c>
       <c r="K10" s="2">
         <v>2281</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
+      <c r="L10" s="2">
+        <v>2445</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2464</v>
+      </c>
+      <c r="N10" s="2">
+        <v>2827</v>
+      </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -745,16 +857,30 @@
       <c r="F11" s="2">
         <v>404</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="G11" s="2">
+        <v>400</v>
+      </c>
+      <c r="H11" s="2">
+        <v>386</v>
+      </c>
+      <c r="I11" s="2">
+        <v>426</v>
+      </c>
+      <c r="J11" s="2">
+        <v>542</v>
+      </c>
       <c r="K11" s="2">
         <v>410</v>
       </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="L11" s="2">
+        <v>382</v>
+      </c>
+      <c r="M11" s="2">
+        <v>404</v>
+      </c>
+      <c r="N11" s="2">
+        <v>406</v>
+      </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -772,16 +898,30 @@
       <c r="F12" s="2">
         <v>19158</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="G12" s="2">
+        <v>19585</v>
+      </c>
+      <c r="H12" s="2">
+        <v>19969</v>
+      </c>
+      <c r="I12" s="2">
+        <v>20731</v>
+      </c>
+      <c r="J12" s="2">
+        <v>22158</v>
+      </c>
       <c r="K12" s="2">
         <v>17476</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
+      <c r="L12" s="2">
+        <v>18293</v>
+      </c>
+      <c r="M12" s="2">
+        <v>17388</v>
+      </c>
+      <c r="N12" s="2">
+        <v>18775</v>
+      </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -799,16 +939,30 @@
       <c r="F13" s="2">
         <v>1581</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="G13" s="2">
+        <v>1896</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1908</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2359</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2663</v>
+      </c>
       <c r="K13" s="2">
         <v>2087</v>
       </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="L13" s="2">
+        <v>2391</v>
+      </c>
+      <c r="M13" s="2">
+        <v>2465</v>
+      </c>
+      <c r="N13" s="2">
+        <v>2948</v>
+      </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -826,16 +980,30 @@
       <c r="F14" s="2">
         <v>24703</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="G14" s="2">
+        <v>27276</v>
+      </c>
+      <c r="H14" s="2">
+        <v>24852</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2811</v>
+      </c>
+      <c r="J14" s="2">
+        <v>32663</v>
+      </c>
       <c r="K14" s="2">
         <v>23707</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="L14" s="2">
+        <v>24537</v>
+      </c>
+      <c r="M14" s="2">
+        <v>24818</v>
+      </c>
+      <c r="N14" s="2">
+        <v>26996</v>
+      </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -853,16 +1021,30 @@
       <c r="F15" s="2">
         <v>2269</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="G15" s="2">
+        <v>2336</v>
+      </c>
+      <c r="H15" s="2">
+        <v>2053</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2243</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2455</v>
+      </c>
       <c r="K15" s="2">
         <v>2099</v>
       </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="L15" s="2">
+        <v>2309</v>
+      </c>
+      <c r="M15" s="2">
+        <v>2419</v>
+      </c>
+      <c r="N15" s="2">
+        <v>2517</v>
+      </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
@@ -880,16 +1062,30 @@
       <c r="F16" s="2">
         <v>9734</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="G16" s="2">
+        <v>9868</v>
+      </c>
+      <c r="H16" s="2">
+        <v>9875</v>
+      </c>
+      <c r="I16" s="2">
+        <v>10546</v>
+      </c>
+      <c r="J16" s="2">
+        <v>10747</v>
+      </c>
       <c r="K16" s="2">
         <v>9421</v>
       </c>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+      <c r="L16" s="2">
+        <v>9532</v>
+      </c>
+      <c r="M16" s="2">
+        <v>9619</v>
+      </c>
+      <c r="N16" s="2">
+        <v>10693</v>
+      </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
@@ -911,37 +1107,37 @@
         <f t="shared" si="0"/>
         <v>2393.5</v>
       </c>
-      <c r="G18" t="e">
+      <c r="G18">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H18" t="e">
+        <v>2626.5</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="I18" t="e">
+        <v>2434.5</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="J18" t="e">
+        <v>2677.5</v>
+      </c>
+      <c r="J18">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>3632.5</v>
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
         <v>2775.5</v>
       </c>
-      <c r="L18" t="e">
+      <c r="L18">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="M18" t="e">
+        <v>3190</v>
+      </c>
+      <c r="M18">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N18" t="e">
+        <v>3301</v>
+      </c>
+      <c r="N18">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
+        <v>3571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix on the data and topic lengths
</commit_message>
<xml_diff>
--- a/data/data_sizes.xlsx
+++ b/data/data_sizes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Uni\TFG\Proyecto-TFG-Reddit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5D74EA-1CA0-4354-B5EC-CC9A61DF9261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BB48E9-B12D-4D35-9EC1-55BC0529A7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="15600" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>abuse</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Median</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
   <dimension ref="B1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="Q10" sqref="C10:Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,7 +1220,7 @@
         <v>8.3441401537407825E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1268,6 +1271,13 @@
       <c r="N18">
         <f t="shared" si="2"/>
         <v>3571</v>
+      </c>
+      <c r="P18" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q18">
+        <f xml:space="preserve"> 24000 * COUNTA(B3:B16)</f>
+        <v>336000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small fix in data_sizes
</commit_message>
<xml_diff>
--- a/data/data_sizes.xlsx
+++ b/data/data_sizes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Uni\TFG\Proyecto-TFG-Reddit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BB48E9-B12D-4D35-9EC1-55BC0529A7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5519A3-12B7-4793-8C39-A33502F74F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,7 +168,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -182,6 +182,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -464,20 +465,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Q18"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q10" sqref="C10:Q10"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C1" s="7" t="s">
         <v>15</v>
       </c>
@@ -493,7 +495,7 @@
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
     </row>
-    <row r="2" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
@@ -534,9 +536,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
         <v>59</v>
@@ -583,9 +586,10 @@
         <v>21.466905187835419</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
         <v>266</v>
@@ -632,7 +636,8 @@
         <v>5.1880674448767836</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -681,9 +686,10 @@
         <v>4.5714285714285712</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2">
         <v>1144</v>
@@ -730,9 +736,10 @@
         <v>1.3901760889712698</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2">
         <v>1817</v>
@@ -779,9 +786,10 @@
         <v>0.94354458248152229</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2">
         <v>1477</v>
@@ -828,9 +836,10 @@
         <v>0.93497993688885428</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2">
         <v>1794</v>
@@ -877,9 +886,10 @@
         <v>0.86617583369423989</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2">
         <v>2101</v>
@@ -926,9 +936,10 @@
         <v>0.6334961066385113</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2">
         <v>6233</v>
@@ -975,9 +986,10 @@
         <v>0.31423072390903023</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2">
         <v>8079</v>
@@ -1024,9 +1036,10 @@
         <v>0.25535446391522232</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C13" s="2">
         <v>10702</v>
@@ -1073,9 +1086,10 @@
         <v>0.19981018032868775</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2">
         <v>9858</v>
@@ -1122,9 +1136,10 @@
         <v>0.16709833737154314</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2">
         <v>17583</v>
@@ -1171,9 +1186,10 @@
         <v>0.10586258154726985</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2">
         <v>22021</v>

</xml_diff>